<commit_message>
Added biological and technical replicate number attributes
</commit_message>
<xml_diff>
--- a/organization/static/siteWide/Metadata_entry_form_V3.xlsx
+++ b/organization/static/siteWide/Metadata_entry_form_V3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="-2440" windowWidth="30060" windowHeight="16340" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="29040" yWindow="-2440" windowWidth="30060" windowHeight="16340" firstSheet="11" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -11524,7 +11524,7 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -20162,7 +20162,7 @@
   <dimension ref="A1:AK104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20294,10 +20294,10 @@
         <v>739</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>129</v>
@@ -24537,7 +24537,9 @@
   </sheetPr>
   <dimension ref="A1:AN104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -24677,10 +24679,10 @@
         <v>739</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>129</v>
@@ -29247,8 +29249,8 @@
   </sheetPr>
   <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -29353,10 +29355,10 @@
         <v>739</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
DCIC ATACSeq changes in Biosample
</commit_message>
<xml_diff>
--- a/organization/static/siteWide/Metadata_entry_form_V3.xlsx
+++ b/organization/static/siteWide/Metadata_entry_form_V3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="-2440" windowWidth="30060" windowHeight="16340" firstSheet="11" activeTab="21"/>
+    <workbookView xWindow="29040" yWindow="-2440" windowWidth="30060" windowHeight="16340" firstSheet="4" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <sheet name="ExperimentSet" sheetId="23" r:id="rId23"/>
     <sheet name="ExperimentSetReplicate" sheetId="24" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="837">
   <si>
     <t>#Field Name:</t>
   </si>
@@ -2053,18 +2053,9 @@
     <t>Chromosome count and any noted rearrangements or copy number variation</t>
   </si>
   <si>
-    <t>karyotype_image</t>
-  </si>
-  <si>
     <t>Item:Image</t>
   </si>
   <si>
-    <t>Image of the karyotype of potentially genomically unstable lines</t>
-  </si>
-  <si>
-    <t>If passage number is more then 10, please supply a karyotype image, or karyotype information from sequencing data.</t>
-  </si>
-  <si>
     <t>morphology_image</t>
   </si>
   <si>
@@ -2555,6 +2546,21 @@
   </si>
   <si>
     <t>Key words that can tag an item - useful for filtering.</t>
+  </si>
+  <si>
+    <t>protocol_classification</t>
+  </si>
+  <si>
+    <t>A classification for a protocol or document that is more specific than it's type.  For example, an Authentication document can be classified as a 'Cell Cycle Authentication' or a Biosample preparation protocol can be classified as 'Tissue Preparation Methods'</t>
+  </si>
+  <si>
+    <t>Choices:['Experiment Authentication', 'Karyotyping Authentication', 'Differentiation Authentication', 'Cell cycle Authentication', 'Instrument Authentication', 'Tissue Preparation Methods']</t>
+  </si>
+  <si>
+    <t>authentication_protocols</t>
+  </si>
+  <si>
+    <t>One or more Protocol objects that are linked to authentication images or documents</t>
   </si>
 </sst>
 </file>
@@ -2593,9 +2599,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11524,13 +11531,12 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="13" max="13" width="20.6640625" customWidth="1"/>
     <col min="14" max="14" width="24.5" customWidth="1"/>
     <col min="15" max="15" width="43.83203125" customWidth="1"/>
   </cols>
@@ -11548,44 +11554,44 @@
       <c r="D1" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>667</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>678</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>176</v>
@@ -11605,16 +11611,16 @@
         <v>645</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
@@ -11629,16 +11635,16 @@
         <v>9</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>668</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>240</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>9</v>
@@ -11661,43 +11667,43 @@
         <v>646</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="O3" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>677</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>177</v>
@@ -11723,25 +11729,25 @@
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>670</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>11</v>
@@ -13792,25 +13798,25 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>688</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>695</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>313</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>16</v>
@@ -13830,25 +13836,25 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>696</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>314</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>17</v>
@@ -13865,22 +13871,22 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>686</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>697</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>315</v>
@@ -13904,13 +13910,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>687</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -13919,10 +13925,10 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>701</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>11</v>
@@ -15364,46 +15370,46 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>717</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>721</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>730</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>176</v>
@@ -15426,25 +15432,25 @@
         <v>171</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>9</v>
@@ -15456,10 +15462,10 @@
         <v>240</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>5</v>
@@ -15473,41 +15479,41 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>177</v>
@@ -15524,7 +15530,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -15533,13 +15539,13 @@
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
@@ -15554,13 +15560,13 @@
         <v>11</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>11</v>
@@ -17602,19 +17608,19 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>730</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>176</v>
@@ -17640,10 +17646,10 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
@@ -17657,20 +17663,20 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>177</v>
@@ -17687,16 +17693,16 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -18821,10 +18827,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18833,7 +18839,7 @@
     <col min="3" max="3" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18849,8 +18855,11 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="2" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -18866,8 +18875,11 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -18881,8 +18893,11 @@
         <v>21</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3" s="2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -18898,8 +18913,11 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4" s="2" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -18916,7 +18934,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -18933,7 +18951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -18950,7 +18968,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -18967,7 +18985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -18984,7 +19002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -19001,7 +19019,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -19018,7 +19036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -19035,7 +19053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -19052,7 +19070,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -19069,7 +19087,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -19086,7 +19104,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -20178,97 +20196,97 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>741</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>753</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>758</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>763</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>662</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>788</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>808</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>170</v>
@@ -20291,7 +20309,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>240</v>
@@ -20303,7 +20321,7 @@
         <v>129</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
@@ -20327,7 +20345,7 @@
         <v>158</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>158</v>
@@ -20369,19 +20387,19 @@
         <v>305</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>171</v>
@@ -20401,100 +20419,100 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>740</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>759</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>764</v>
-      </c>
       <c r="O3" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>772</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>779</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="W3" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>789</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="AE3" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="AF3" s="1" t="s">
-        <v>804</v>
-      </c>
       <c r="AG3" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>172</v>
@@ -20532,19 +20550,19 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>664</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>11</v>
@@ -20553,7 +20571,7 @@
         <v>11</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>11</v>
@@ -20574,10 +20592,10 @@
         <v>11</v>
       </c>
       <c r="W4" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>787</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>11</v>
@@ -20604,7 +20622,7 @@
         <v>11</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="AH4" s="1" t="s">
         <v>11</v>
@@ -24554,106 +24572,106 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>741</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>753</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>758</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>763</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>662</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>788</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>808</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>170</v>
@@ -24676,7 +24694,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>240</v>
@@ -24688,7 +24706,7 @@
         <v>129</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
@@ -24712,7 +24730,7 @@
         <v>158</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>158</v>
@@ -24754,7 +24772,7 @@
         <v>305</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>9</v>
@@ -24763,19 +24781,19 @@
         <v>9</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>171</v>
@@ -24795,109 +24813,109 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>740</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>759</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>764</v>
-      </c>
       <c r="O3" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>772</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>779</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="W3" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>789</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="AF3" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="AI3" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="AG3" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>804</v>
-      </c>
       <c r="AJ3" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="AL3" s="1" t="s">
         <v>172</v>
@@ -24935,19 +24953,19 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>664</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>11</v>
@@ -24956,7 +24974,7 @@
         <v>11</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>11</v>
@@ -24977,10 +24995,10 @@
         <v>11</v>
       </c>
       <c r="W4" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>787</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>11</v>
@@ -25016,7 +25034,7 @@
         <v>11</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="AK4" s="1" t="s">
         <v>11</v>
@@ -29249,7 +29267,7 @@
   </sheetPr>
   <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -29266,70 +29284,70 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>741</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>753</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>662</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>831</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>808</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>170</v>
@@ -29352,7 +29370,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>240</v>
@@ -29364,13 +29382,13 @@
         <v>129</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>158</v>
@@ -29403,19 +29421,19 @@
         <v>305</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>171</v>
@@ -29435,73 +29453,73 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>740</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>832</v>
-      </c>
       <c r="W3" s="1" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>172</v>
@@ -29539,7 +29557,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
@@ -29548,7 +29566,7 @@
         <v>11</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>11</v>
@@ -29569,7 +29587,7 @@
         <v>11</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>11</v>
@@ -29584,7 +29602,7 @@
         <v>11</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>11</v>
@@ -32663,10 +32681,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>172</v>
@@ -33453,10 +33471,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>172</v>

</xml_diff>